<commit_message>
Update Entry Date field in HSI Review sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI_Review.xlsx
+++ b/Input documents/HSI_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">29/01/2019</t>
+    <t xml:space="preserve">29/01/2020</t>
   </si>
   <si>
     <t xml:space="preserve">A.Ali</t>
@@ -117,39 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">Page 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of document must be changed from Draft to Proposed and then Releases after accomplishing cross review on it. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redundancy in Version field besides Date in header table. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is no Reference table for the reference document , even HSI should have one and the reference is the customer Requirement for the product </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 5</t>
   </si>
   <si>
     <r>
@@ -160,7 +127,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">System Block Diagram shall be updated to match customer specification defined in CRS , as there’s no mentioned specification states that there’s 3 LEDs  and the arrow </t>
+      <t xml:space="preserve">Status of document must be changed from Draft to Proposed and then Released after accomplishing cross review on it. 
+I </t>
     </r>
     <r>
       <rPr>
@@ -169,18 +137,32 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">connected </t>
+      <t xml:space="preserve">expect if cross review was done by another team member , the status of document should be Released. </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">between push button and Microcontroller should be an input not output. </t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redundancy in Version field besides Date in header table. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no Reference table for the reference document , even HSI should have one and the reference is the customer Requirement for the product </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Block Diagram shall be updated to match customer specification defined in CRS , as there’s no mentioned specification states that there’s 3 LEDs  and the arrow connected between push button and Microcontroller should be an input not output. </t>
   </si>
   <si>
     <t xml:space="preserve">Page 6</t>
@@ -526,7 +508,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,7 +532,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -742,7 +724,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
   </cols>
@@ -984,10 +966,10 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
@@ -1028,7 +1010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -1054,8 +1036,8 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>33</v>
+      <c r="A3" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>27</v>
@@ -1067,10 +1049,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>34</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>35</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22" t="s">
@@ -1078,24 +1060,24 @@
       </c>
       <c r="I3" s="22"/>
     </row>
-    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22" t="s">
@@ -1103,27 +1085,27 @@
       </c>
       <c r="I4" s="22"/>
       <c r="K4" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="22" t="s">
@@ -1133,22 +1115,22 @@
     </row>
     <row r="6" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22" t="s">
@@ -1158,22 +1140,22 @@
     </row>
     <row r="7" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22" t="s">
@@ -1185,7 +1167,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" s="18"/>
@@ -1195,11 +1177,11 @@
       <c r="H8" s="22"/>
       <c r="I8" s="20"/>
       <c r="K8" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
       <c r="D9" s="18"/>
@@ -1231,10 +1213,10 @@
       <c r="H11" s="22"/>
       <c r="I11" s="20"/>
       <c r="K11" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,10 +1230,10 @@
       <c r="H12" s="22"/>
       <c r="I12" s="20"/>
       <c r="K12" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,7 +1625,7 @@
   </sheetData>
   <conditionalFormatting sqref="G1">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>#REF!</formula>
+      <formula>#ref!</formula>
     </cfRule>
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$G$3</formula>
@@ -1657,7 +1639,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
     <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>#REF!</formula>
+      <formula>#ref!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Add new revies points of HSI document for week 2 Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI_Review.xlsx
+++ b/Input documents/HSI_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -123,7 +123,10 @@
 I expect if cross review was done by another team member , the status of document should be Released. </t>
   </si>
   <si>
-    <t xml:space="preserve">Open</t>
+    <t xml:space="preserve">Accepted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">All pages</t>
@@ -160,7 +163,21 @@
 - Need to review HSI requirements again and add a related HW requirements from the system level prospective. </t>
   </si>
   <si>
-    <t xml:space="preserve">Resolved</t>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version Date format in header table is different from the Date field in Release Table in page 2 , plaese apply a unique Date format for all date fields , also HSI document stands for Hardware Software Interface. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Pin Mode Representation table, missed to add the sufficient pins to some components ex: Motor (has 2 DIO pins not one) , Also GND , VCC pins should be added as a used pins. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redundant requirements between Functional Requirements and Pin Mode Representation table. 
+As Functional requirements should describe a feature will be implemented in the system from the HW prospective , ask this question  (What shall be considered when implement a HW for this feature?) . 
+Ex: we you’ve a device or external peripheral works on 16 MHz clock and your selected Microcontroller has an internal oscillator 8 MHz , what you’ll need to consider in your HW implementation to overcome this issue. </t>
   </si>
   <si>
     <t xml:space="preserve">Decision </t>
@@ -179,14 +196,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]General"/>
     <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
     <numFmt numFmtId="168" formatCode="@"/>
+    <numFmt numFmtId="169" formatCode="[$-409]MM/DD/YY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -231,6 +249,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -415,7 +439,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -512,6 +536,18 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -532,7 +568,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,7 +576,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -696,7 +732,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
   </cols>
@@ -938,10 +974,10 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
@@ -949,7 +985,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
   </cols>
   <sheetData>
@@ -982,7 +1019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -1001,9 +1038,11 @@
       <c r="F2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H2" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I2" s="22"/>
     </row>
@@ -1021,16 +1060,21 @@
         <v>29</v>
       </c>
       <c r="E3" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22" t="s">
+      <c r="I3" s="22"/>
+      <c r="K3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
@@ -1046,18 +1090,20 @@
         <v>29</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="22"/>
+        <v>37</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H4" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="22"/>
       <c r="K4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1074,14 +1120,16 @@
         <v>29</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="22"/>
+        <v>40</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H5" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="22"/>
     </row>
@@ -1099,14 +1147,16 @@
         <v>29</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H6" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="20"/>
     </row>
@@ -1124,54 +1174,98 @@
         <v>29</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H7" s="22" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="I7" s="20"/>
       <c r="K7" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="n">
+        <v>44014</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>47</v>
+      </c>
       <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="H8" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="I8" s="20"/>
       <c r="K8" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="25" t="n">
+        <v>44014</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>48</v>
+      </c>
       <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
+    <row r="10" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="25" t="n">
+        <v>44014</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="I10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,10 +1279,10 @@
       <c r="H11" s="22"/>
       <c r="I11" s="20"/>
       <c r="K11" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,10 +1296,10 @@
       <c r="H12" s="22"/>
       <c r="I12" s="20"/>
       <c r="K12" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1242,356 +1336,356 @@
       <c r="I15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
-      <c r="I16" s="29"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="29"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="28"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
-      <c r="I18" s="29"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="29"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="29"/>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="29"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="34"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="29"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="29"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
-      <c r="I24" s="29"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
-      <c r="I25" s="29"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
-      <c r="I26" s="29"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
-      <c r="I27" s="29"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="31"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
-      <c r="I28" s="29"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="31"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
-      <c r="I29" s="29"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
-      <c r="I30" s="29"/>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="32"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
-      <c r="I31" s="29"/>
+      <c r="I31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="31"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
-      <c r="I32" s="29"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="31"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
-      <c r="I33" s="29"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
-      <c r="I34" s="29"/>
+      <c r="I34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="31"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
-      <c r="I35" s="29"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="31"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="29"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="31"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
-      <c r="I37" s="29"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="31"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="29"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="31"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="34"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="29"/>
+      <c r="I39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="31"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
-      <c r="I40" s="29"/>
+      <c r="I40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="31"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="34"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
-      <c r="I41" s="29"/>
+      <c r="I41" s="32"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="31"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="34"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
-      <c r="I42" s="29"/>
+      <c r="I42" s="32"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="31"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="34"/>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
-      <c r="I43" s="29"/>
+      <c r="I43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="31"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="34"/>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
-      <c r="I44" s="29"/>
+      <c r="I44" s="32"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="31"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="34"/>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
-      <c r="I45" s="29"/>
+      <c r="I45" s="32"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="31"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="34"/>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
-      <c r="I46" s="29"/>
+      <c r="I46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="31"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="34"/>
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
-      <c r="I47" s="29"/>
+      <c r="I47" s="32"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1614,13 +1708,17 @@
       <formula>#ref!</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1047" type="list">
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1 G8:G1047" type="list">
       <formula1>$K$4:$K$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1047" type="list">
       <formula1>$K$7:$K$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G7" type="list">
+      <formula1>$K$3:$K$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>